<commit_message>
feat: LootTable and CharacterStats
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/_Enums.xlsx
+++ b/Tools/Luban/Datas/_Enums.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Godot\FlowerRPGGD\Tools\Luban\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DC03CA-5EA7-491C-B997-57AEEA4932E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDDDEFC-0968-45D8-AEC9-49B699DA42B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>##var</t>
   </si>
@@ -103,6 +103,38 @@
   </si>
   <si>
     <t>Speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items.ItemType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items.Rarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Legendary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.149999999999999" x14ac:dyDescent="0.45"/>
@@ -599,6 +631,48 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:L1"/>

</xml_diff>